<commit_message>
Changes in code: now choosing the correct Id if one is in brackets, according to the required record type. Also migration script printing was realized.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -134,7 +134,7 @@
   </si>
   <si>
     <t>1548
-1549
+1549 (8888)
 1550</t>
   </si>
   <si>
@@ -230,7 +230,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -450,17 +450,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -488,10 +488,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -739,12 +739,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1031,7 +1031,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1059,10 +1059,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1469,7 +1469,7 @@
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="5">
-        <v>43342</v>
+        <v>43343</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>

</xml_diff>